<commit_message>
grab empty days from sheets
</commit_message>
<xml_diff>
--- a/Copy of 06-16-24 to 06-22-24 Milwaukee Schedule.xlsx
+++ b/Copy of 06-16-24 to 06-22-24 Milwaukee Schedule.xlsx
@@ -660,11 +660,7 @@
     </row>
     <row r="8">
       <c r="A8" t="inlineStr"/>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>FATHER'S DAY</t>
-        </is>
-      </c>
+      <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr"/>
       <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">

</xml_diff>